<commit_message>
Programme de création de pattern et pattern comparaison pgg connectés à la bdd
</commit_message>
<xml_diff>
--- a/PPG_data_combined.xlsx
+++ b/PPG_data_combined.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cresp\OneDrive\Documents\Sleevy\Sleevy2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2857479F-260E-45E3-8F35-0D5F45B3D1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC9A16E-F267-4A4A-9E64-B339AED17B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,20 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -485,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1204"/>
+  <dimension ref="A1:T1206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A1176" workbookViewId="0">
+      <selection activeCell="P1206" sqref="P1206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -47287,6 +47300,12 @@
       </c>
       <c r="P1204">
         <v>71</v>
+      </c>
+    </row>
+    <row r="1206" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="P1206">
+        <f>AVERAGE(P2:P1204)</f>
+        <v>69.411471321695757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fonction pattern et comparaison good
</commit_message>
<xml_diff>
--- a/PPG_data_combined.xlsx
+++ b/PPG_data_combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cresp\OneDrive\Documents\Sleevy\Sleevy2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC9A16E-F267-4A4A-9E64-B339AED17B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5671433C-072A-4F3D-B06E-1186F4370357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -498,9 +498,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1206"/>
+  <dimension ref="A1:T1204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1176" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A1194" workbookViewId="0">
       <selection activeCell="P1206" sqref="P1206"/>
     </sheetView>
   </sheetViews>
@@ -47300,12 +47300,6 @@
       </c>
       <c r="P1204">
         <v>71</v>
-      </c>
-    </row>
-    <row r="1206" spans="15:16" x14ac:dyDescent="0.45">
-      <c r="P1206">
-        <f>AVERAGE(P2:P1204)</f>
-        <v>69.411471321695757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>